<commit_message>
Simulation 20nodes fix (#3)
ran sanity checks
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="tests" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
-    <sheet name="ht paths" sheetId="3" r:id="rId3"/>
+    <sheet name="tests_8nodes" sheetId="1" r:id="rId1"/>
+    <sheet name="test_20nodes" sheetId="4" r:id="rId2"/>
+    <sheet name="data" sheetId="2" r:id="rId3"/>
+    <sheet name="ht paths" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="130">
   <si>
     <t>Battery Front</t>
   </si>
@@ -335,6 +336,87 @@
   </si>
   <si>
     <t>Platem</t>
+  </si>
+  <si>
+    <t>ESC_Mount</t>
+  </si>
+  <si>
+    <t>Plate Top</t>
+  </si>
+  <si>
+    <t>Plate Middle</t>
+  </si>
+  <si>
+    <t>Plate Bottom</t>
+  </si>
+  <si>
+    <t>Top Shell External</t>
+  </si>
+  <si>
+    <t>Bottom Shell Internal</t>
+  </si>
+  <si>
+    <t>Bottom Shell External</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emissivity </t>
+  </si>
+  <si>
+    <t>Thermal conductivity of shell (k) : 1 W/mk (CFRP),</t>
+  </si>
+  <si>
+    <t>Emissivity (Shell Int)</t>
+  </si>
+  <si>
+    <t>Thermal conductivity of shell (k) : 1 W/mk, (CFRP)</t>
+  </si>
+  <si>
+    <t>Running Time (T) : 14 days</t>
+  </si>
+  <si>
+    <t>Initial Temperature: 305 K (32C),</t>
+  </si>
+  <si>
+    <t>Ambient temperature: 287.34K (14C) (Temp at alt 0.125 km)</t>
+  </si>
+  <si>
+    <t>As we can see when we reduce the emissivity of the internal shell the temperature inside the nacelle rises, the ambient temperature was set on the basis of altitude we were simulating at through an automated excel file and we took initial temperature higher than the ambient temp to avoid a theral shock to the the solver which is a issue we've been facing a lot since the start of scale up of the number of nodes</t>
+  </si>
+  <si>
+    <t>Thermal conductivity of shell (k)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As we can see there is a drastic decrease when we increased the thermal conductivity but the results are more or less similar to our normal conduction which indicated that where a very good insulator is bad for our nacelle a very good conductor is not something we need too, there were observations of thermal shock in esc in day 1 most probably due to such low mC but later it retained steady state </t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Thickness of Shell</t>
+  </si>
+  <si>
+    <t>As we can observe when we increase the thickness the temp inside the nacelle increases a striking difference between internal and external shell temp is observed making it quite clear that as we increase our thickness nacelle insides becomes hotter</t>
+  </si>
+  <si>
+    <t>Result 1 – Effect of forced convection</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>As we can observe there is a decrease of around 10 degrees in every component when we introduced a velocity of 8m/s</t>
+  </si>
+  <si>
+    <t>Result 2 – Aerogel Induced working Temperatures</t>
+  </si>
+  <si>
+    <t>Thermal conductivity of shell (k) : 0.0015 W/mk, (CFRP)</t>
+  </si>
+  <si>
+    <t>Emissivity of shell : 0.2</t>
+  </si>
+  <si>
+    <t>Even though the temp is abnormally high it completely makes sense we increased the thickness hence reducing the conduction btw internal and external shell, we reduced the emissivity decreasing the ability of other components to pass on heat to the internal shell for dissipation to the atmosphere and we reduced the thermal conductivity which makes it even more difficult for the heat retained by internal shell to be passed on to external shell hence leading to extreme temp inside the nacelle whereas the outside is cool due to external convection and radiation</t>
   </si>
 </sst>
 </file>
@@ -424,7 +506,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -489,11 +571,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -547,17 +642,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -577,19 +670,49 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -872,13 +995,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P182"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="I175" sqref="I175"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54:C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="77.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="84.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" customWidth="1"/>
@@ -897,14 +1020,14 @@
     <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E2" s="9" t="s">
+    <row r="2" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E2" s="42" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="8" t="s">
-        <v>13</v>
+        <v>111</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -922,19 +1045,19 @@
       <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="38" t="s">
+      <c r="F4" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
@@ -982,25 +1105,25 @@
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
       <c r="E6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="27">
+        <v>110</v>
+      </c>
+      <c r="F6" s="30">
         <v>0.05</v>
       </c>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27">
+      <c r="G6" s="30"/>
+      <c r="H6" s="30">
         <v>0.75</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="30"/>
       <c r="J6" s="32"/>
-      <c r="K6" s="27">
+      <c r="K6" s="30">
         <v>0.05</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27">
+      <c r="L6" s="30"/>
+      <c r="M6" s="30">
         <v>0.75</v>
       </c>
-      <c r="N6" s="27"/>
+      <c r="N6" s="30"/>
       <c r="O6" s="35"/>
       <c r="P6" s="36"/>
     </row>
@@ -1368,19 +1491,19 @@
       <c r="E20" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="38" t="s">
+      <c r="F20" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="10"/>
-      <c r="K20" s="38" t="s">
+      <c r="K20" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="38"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
@@ -1430,23 +1553,23 @@
       <c r="E22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="30">
         <v>1E-3</v>
       </c>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27">
+      <c r="G22" s="30"/>
+      <c r="H22" s="30">
         <v>400</v>
       </c>
-      <c r="I22" s="27"/>
+      <c r="I22" s="30"/>
       <c r="J22" s="32"/>
-      <c r="K22" s="27">
+      <c r="K22" s="30">
         <v>1E-3</v>
       </c>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27">
+      <c r="L22" s="30"/>
+      <c r="M22" s="30">
         <v>400</v>
       </c>
-      <c r="N22" s="27"/>
+      <c r="N22" s="30"/>
       <c r="O22" s="35"/>
       <c r="P22" s="36"/>
     </row>
@@ -1814,19 +1937,19 @@
       <c r="E36" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="38" t="s">
+      <c r="F36" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="38"/>
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
       <c r="J36" s="10"/>
-      <c r="K36" s="38" t="s">
+      <c r="K36" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="38"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
@@ -1874,25 +1997,25 @@
       <c r="B38" s="31"/>
       <c r="C38" s="31"/>
       <c r="E38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="27">
+        <v>120</v>
+      </c>
+      <c r="F38" s="30">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27">
+      <c r="G38" s="30"/>
+      <c r="H38" s="30">
         <v>0.05</v>
       </c>
-      <c r="I38" s="27"/>
+      <c r="I38" s="30"/>
       <c r="J38" s="32"/>
-      <c r="K38" s="27">
+      <c r="K38" s="30">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27">
+      <c r="L38" s="30"/>
+      <c r="M38" s="30">
         <v>0.05</v>
       </c>
-      <c r="N38" s="27"/>
+      <c r="N38" s="30"/>
       <c r="O38" s="35"/>
       <c r="P38" s="36"/>
     </row>
@@ -2265,19 +2388,19 @@
       <c r="E53" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F53" s="38" t="s">
+      <c r="F53" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
       <c r="J53" s="10"/>
-      <c r="K53" s="38" t="s">
+      <c r="K53" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L53" s="38"/>
-      <c r="M53" s="38"/>
-      <c r="N53" s="38"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="29"/>
+      <c r="N53" s="29"/>
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
@@ -2327,23 +2450,23 @@
       <c r="E55" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F55" s="27" t="s">
+      <c r="F55" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27" t="s">
+      <c r="G55" s="30"/>
+      <c r="H55" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="I55" s="27"/>
+      <c r="I55" s="30"/>
       <c r="J55" s="32"/>
-      <c r="K55" s="27" t="s">
+      <c r="K55" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="L55" s="27"/>
-      <c r="M55" s="27" t="s">
+      <c r="L55" s="30"/>
+      <c r="M55" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="N55" s="27"/>
+      <c r="N55" s="30"/>
       <c r="O55" s="35"/>
       <c r="P55" s="36"/>
     </row>
@@ -2716,19 +2839,19 @@
       <c r="E70" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F70" s="38" t="s">
+      <c r="F70" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G70" s="38"/>
-      <c r="H70" s="38"/>
-      <c r="I70" s="38"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
       <c r="J70" s="10"/>
-      <c r="K70" s="38" t="s">
+      <c r="K70" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L70" s="38"/>
-      <c r="M70" s="38"/>
-      <c r="N70" s="38"/>
+      <c r="L70" s="29"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="29"/>
       <c r="O70" s="1"/>
       <c r="P70" s="1"/>
     </row>
@@ -2778,23 +2901,23 @@
       <c r="E72" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F72" s="27" t="s">
+      <c r="F72" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27" t="s">
+      <c r="G72" s="30"/>
+      <c r="H72" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I72" s="27"/>
+      <c r="I72" s="30"/>
       <c r="J72" s="32"/>
-      <c r="K72" s="27" t="s">
+      <c r="K72" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="L72" s="27"/>
-      <c r="M72" s="27" t="s">
+      <c r="L72" s="30"/>
+      <c r="M72" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="N72" s="27"/>
+      <c r="N72" s="30"/>
       <c r="O72" s="35"/>
       <c r="P72" s="36"/>
     </row>
@@ -3183,19 +3306,19 @@
       <c r="E88" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F88" s="38" t="s">
+      <c r="F88" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="G88" s="38"/>
-      <c r="H88" s="38"/>
-      <c r="I88" s="38"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="29"/>
       <c r="J88" s="10"/>
-      <c r="K88" s="38" t="s">
+      <c r="K88" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="L88" s="38"/>
-      <c r="M88" s="38"/>
-      <c r="N88" s="38"/>
+      <c r="L88" s="29"/>
+      <c r="M88" s="29"/>
+      <c r="N88" s="29"/>
       <c r="O88" s="1"/>
       <c r="P88" s="1"/>
     </row>
@@ -3245,23 +3368,23 @@
       <c r="E90" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F90" s="27" t="s">
+      <c r="F90" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="G90" s="27"/>
-      <c r="H90" s="27" t="s">
+      <c r="G90" s="30"/>
+      <c r="H90" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="I90" s="27"/>
+      <c r="I90" s="30"/>
       <c r="J90" s="32"/>
-      <c r="K90" s="27" t="s">
+      <c r="K90" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="L90" s="27"/>
-      <c r="M90" s="27" t="s">
+      <c r="L90" s="30"/>
+      <c r="M90" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="N90" s="27"/>
+      <c r="N90" s="30"/>
       <c r="O90" s="35"/>
       <c r="P90" s="36"/>
     </row>
@@ -3618,17 +3741,17 @@
       <c r="E104" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F104" s="38" t="s">
+      <c r="F104" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="G104" s="38"/>
-      <c r="H104" s="38"/>
-      <c r="I104" s="38"/>
-      <c r="J104" s="38"/>
-      <c r="K104" s="38"/>
-      <c r="L104" s="38"/>
-      <c r="M104" s="38"/>
-      <c r="N104" s="38"/>
+      <c r="G104" s="29"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="29"/>
+      <c r="J104" s="29"/>
+      <c r="K104" s="29"/>
+      <c r="L104" s="29"/>
+      <c r="M104" s="29"/>
+      <c r="N104" s="29"/>
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
     </row>
@@ -3678,23 +3801,23 @@
       <c r="E106" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F106" s="27" t="s">
+      <c r="F106" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="G106" s="27"/>
-      <c r="H106" s="27" t="s">
+      <c r="G106" s="30"/>
+      <c r="H106" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="I106" s="27"/>
+      <c r="I106" s="30"/>
       <c r="J106" s="32"/>
-      <c r="K106" s="27" t="s">
+      <c r="K106" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="L106" s="27"/>
-      <c r="M106" s="27" t="s">
+      <c r="L106" s="30"/>
+      <c r="M106" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="N106" s="27"/>
+      <c r="N106" s="30"/>
       <c r="O106" s="35"/>
       <c r="P106" s="36"/>
     </row>
@@ -4072,12 +4195,12 @@
       <c r="E123" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F123" s="38" t="s">
+      <c r="F123" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="G123" s="38"/>
-      <c r="H123" s="38"/>
-      <c r="I123" s="38"/>
+      <c r="G123" s="29"/>
+      <c r="H123" s="29"/>
+      <c r="I123" s="29"/>
       <c r="J123" s="10"/>
       <c r="K123" s="13" t="s">
         <v>61</v>
@@ -4134,23 +4257,23 @@
       <c r="E125" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F125" s="27">
+      <c r="F125" s="30">
         <v>0.05</v>
       </c>
-      <c r="G125" s="27"/>
-      <c r="H125" s="27">
+      <c r="G125" s="30"/>
+      <c r="H125" s="30">
         <v>0.75</v>
       </c>
-      <c r="I125" s="27"/>
+      <c r="I125" s="30"/>
       <c r="J125" s="32"/>
-      <c r="K125" s="27">
+      <c r="K125" s="30">
         <v>0.05</v>
       </c>
-      <c r="L125" s="27"/>
-      <c r="M125" s="27">
+      <c r="L125" s="30"/>
+      <c r="M125" s="30">
         <v>0.75</v>
       </c>
-      <c r="N125" s="27"/>
+      <c r="N125" s="30"/>
       <c r="O125" s="35" t="s">
         <v>72</v>
       </c>
@@ -4539,45 +4662,45 @@
       <c r="E139" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F139" s="30" t="s">
+      <c r="F139" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G139" s="30"/>
-      <c r="H139" s="30"/>
-      <c r="I139" s="30"/>
-      <c r="K139" s="30" t="s">
+      <c r="G139" s="37"/>
+      <c r="H139" s="37"/>
+      <c r="I139" s="37"/>
+      <c r="K139" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="L139" s="30"/>
-      <c r="M139" s="30"/>
-      <c r="N139" s="30"/>
+      <c r="L139" s="37"/>
+      <c r="M139" s="37"/>
+      <c r="N139" s="37"/>
     </row>
     <row r="140" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E140" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F140" s="30"/>
-      <c r="G140" s="30"/>
-      <c r="H140" s="30"/>
-      <c r="I140" s="30"/>
-      <c r="K140" s="30"/>
-      <c r="L140" s="30"/>
-      <c r="M140" s="30"/>
-      <c r="N140" s="30"/>
+      <c r="F140" s="37"/>
+      <c r="G140" s="37"/>
+      <c r="H140" s="37"/>
+      <c r="I140" s="37"/>
+      <c r="K140" s="37"/>
+      <c r="L140" s="37"/>
+      <c r="M140" s="37"/>
+      <c r="N140" s="37"/>
     </row>
     <row r="141" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="E141" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F141" s="30"/>
-      <c r="G141" s="30"/>
-      <c r="H141" s="30"/>
-      <c r="I141" s="30"/>
+      <c r="F141" s="37"/>
+      <c r="G141" s="37"/>
+      <c r="H141" s="37"/>
+      <c r="I141" s="37"/>
       <c r="J141" s="1"/>
-      <c r="K141" s="30"/>
-      <c r="L141" s="30"/>
-      <c r="M141" s="30"/>
-      <c r="N141" s="30"/>
+      <c r="K141" s="37"/>
+      <c r="L141" s="37"/>
+      <c r="M141" s="37"/>
+      <c r="N141" s="37"/>
       <c r="O141" s="1"/>
       <c r="P141" s="1"/>
     </row>
@@ -4627,23 +4750,23 @@
       <c r="E143" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F143" s="27" t="s">
+      <c r="F143" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="G143" s="27"/>
-      <c r="H143" s="27" t="s">
+      <c r="G143" s="30"/>
+      <c r="H143" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="I143" s="27"/>
+      <c r="I143" s="30"/>
       <c r="J143" s="32"/>
-      <c r="K143" s="27" t="s">
+      <c r="K143" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="L143" s="27"/>
-      <c r="M143" s="27" t="s">
+      <c r="L143" s="30"/>
+      <c r="M143" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="N143" s="27"/>
+      <c r="N143" s="30"/>
       <c r="O143" s="35"/>
       <c r="P143" s="36"/>
     </row>
@@ -5027,45 +5150,45 @@
       <c r="E156" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F156" s="30" t="s">
+      <c r="F156" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G156" s="30"/>
-      <c r="H156" s="30"/>
-      <c r="I156" s="30"/>
-      <c r="K156" s="30" t="s">
+      <c r="G156" s="37"/>
+      <c r="H156" s="37"/>
+      <c r="I156" s="37"/>
+      <c r="K156" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="L156" s="30"/>
-      <c r="M156" s="30"/>
-      <c r="N156" s="30"/>
+      <c r="L156" s="37"/>
+      <c r="M156" s="37"/>
+      <c r="N156" s="37"/>
     </row>
     <row r="157" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E157" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F157" s="30"/>
-      <c r="G157" s="30"/>
-      <c r="H157" s="30"/>
-      <c r="I157" s="30"/>
-      <c r="K157" s="30"/>
-      <c r="L157" s="30"/>
-      <c r="M157" s="30"/>
-      <c r="N157" s="30"/>
+      <c r="F157" s="37"/>
+      <c r="G157" s="37"/>
+      <c r="H157" s="37"/>
+      <c r="I157" s="37"/>
+      <c r="K157" s="37"/>
+      <c r="L157" s="37"/>
+      <c r="M157" s="37"/>
+      <c r="N157" s="37"/>
     </row>
     <row r="158" spans="1:16" ht="18.75" x14ac:dyDescent="0.25">
       <c r="E158" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="F158" s="30"/>
-      <c r="G158" s="30"/>
-      <c r="H158" s="30"/>
-      <c r="I158" s="30"/>
+      <c r="F158" s="37"/>
+      <c r="G158" s="37"/>
+      <c r="H158" s="37"/>
+      <c r="I158" s="37"/>
       <c r="J158" s="1"/>
-      <c r="K158" s="30"/>
-      <c r="L158" s="30"/>
-      <c r="M158" s="30"/>
-      <c r="N158" s="30"/>
+      <c r="K158" s="37"/>
+      <c r="L158" s="37"/>
+      <c r="M158" s="37"/>
+      <c r="N158" s="37"/>
       <c r="O158" s="1"/>
       <c r="P158" s="1"/>
     </row>
@@ -5078,23 +5201,23 @@
       <c r="E159" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F159" s="37" t="s">
+      <c r="F159" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="G159" s="37"/>
-      <c r="H159" s="37" t="s">
+      <c r="G159" s="39"/>
+      <c r="H159" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="I159" s="37"/>
+      <c r="I159" s="39"/>
       <c r="J159" s="32"/>
-      <c r="K159" s="37" t="s">
+      <c r="K159" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="L159" s="37"/>
-      <c r="M159" s="37" t="s">
+      <c r="L159" s="39"/>
+      <c r="M159" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="N159" s="37"/>
+      <c r="N159" s="39"/>
       <c r="O159" s="33" t="s">
         <v>12</v>
       </c>
@@ -5107,19 +5230,19 @@
       <c r="E160" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F160" s="27" t="s">
+      <c r="F160" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="G160" s="27"/>
-      <c r="H160" s="27"/>
-      <c r="I160" s="27"/>
+      <c r="G160" s="30"/>
+      <c r="H160" s="30"/>
+      <c r="I160" s="30"/>
       <c r="J160" s="32"/>
-      <c r="K160" s="27" t="s">
+      <c r="K160" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="L160" s="27"/>
-      <c r="M160" s="27"/>
-      <c r="N160" s="27"/>
+      <c r="L160" s="30"/>
+      <c r="M160" s="30"/>
+      <c r="N160" s="30"/>
       <c r="O160" s="35"/>
       <c r="P160" s="36"/>
     </row>
@@ -5130,25 +5253,25 @@
       <c r="E161" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F161" s="28">
+      <c r="F161" s="38">
         <v>342.04</v>
       </c>
-      <c r="G161" s="28"/>
-      <c r="H161" s="29">
+      <c r="G161" s="38"/>
+      <c r="H161" s="40">
         <f>F161-273.15</f>
         <v>68.890000000000043</v>
       </c>
-      <c r="I161" s="29"/>
+      <c r="I161" s="40"/>
       <c r="J161" s="32"/>
-      <c r="K161" s="28">
+      <c r="K161" s="38">
         <v>322.26</v>
       </c>
-      <c r="L161" s="28"/>
-      <c r="M161" s="29">
+      <c r="L161" s="38"/>
+      <c r="M161" s="40">
         <f>K161-273.15</f>
         <v>49.110000000000014</v>
       </c>
-      <c r="N161" s="29"/>
+      <c r="N161" s="40"/>
       <c r="O161" s="35"/>
       <c r="P161" s="36"/>
     </row>
@@ -5159,25 +5282,25 @@
       <c r="E162" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F162" s="28">
+      <c r="F162" s="38">
         <v>319.17</v>
       </c>
-      <c r="G162" s="28"/>
-      <c r="H162" s="29">
+      <c r="G162" s="38"/>
+      <c r="H162" s="40">
         <f>F162-273.15</f>
         <v>46.020000000000039</v>
       </c>
-      <c r="I162" s="29"/>
+      <c r="I162" s="40"/>
       <c r="J162" s="32"/>
-      <c r="K162" s="28">
+      <c r="K162" s="38">
         <v>301.64999999999998</v>
       </c>
-      <c r="L162" s="28"/>
-      <c r="M162" s="29">
+      <c r="L162" s="38"/>
+      <c r="M162" s="40">
         <f>K162-273.15</f>
         <v>28.5</v>
       </c>
-      <c r="N162" s="29"/>
+      <c r="N162" s="40"/>
       <c r="O162" s="35"/>
       <c r="P162" s="36"/>
     </row>
@@ -5188,25 +5311,25 @@
       <c r="E163" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F163" s="28">
+      <c r="F163" s="38">
         <v>317.06</v>
       </c>
-      <c r="G163" s="28"/>
-      <c r="H163" s="29">
+      <c r="G163" s="38"/>
+      <c r="H163" s="40">
         <f t="shared" ref="H163:H170" si="37">F163-273.15</f>
         <v>43.910000000000025</v>
       </c>
-      <c r="I163" s="29"/>
+      <c r="I163" s="40"/>
       <c r="J163" s="32"/>
-      <c r="K163" s="28">
+      <c r="K163" s="38">
         <v>298.48</v>
       </c>
-      <c r="L163" s="28"/>
-      <c r="M163" s="29">
+      <c r="L163" s="38"/>
+      <c r="M163" s="40">
         <f t="shared" ref="M163" si="38">K163-273.15</f>
         <v>25.330000000000041</v>
       </c>
-      <c r="N163" s="29"/>
+      <c r="N163" s="40"/>
       <c r="O163" s="35"/>
       <c r="P163" s="36"/>
     </row>
@@ -5217,24 +5340,24 @@
       <c r="E164" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F164" s="28" t="s">
+      <c r="F164" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="G164" s="28"/>
-      <c r="H164" s="29" t="s">
+      <c r="G164" s="38"/>
+      <c r="H164" s="40" t="s">
         <v>73</v>
       </c>
-      <c r="I164" s="29"/>
+      <c r="I164" s="40"/>
       <c r="J164" s="32"/>
-      <c r="K164" s="28">
+      <c r="K164" s="38">
         <v>378.41</v>
       </c>
-      <c r="L164" s="28"/>
-      <c r="M164" s="29">
+      <c r="L164" s="38"/>
+      <c r="M164" s="40">
         <f>K164-273.15</f>
         <v>105.26000000000005</v>
       </c>
-      <c r="N164" s="29"/>
+      <c r="N164" s="40"/>
       <c r="O164" s="35"/>
       <c r="P164" s="36"/>
     </row>
@@ -5245,25 +5368,25 @@
       <c r="E165" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F165" s="28">
+      <c r="F165" s="38">
         <v>372.15</v>
       </c>
-      <c r="G165" s="28"/>
-      <c r="H165" s="29">
+      <c r="G165" s="38"/>
+      <c r="H165" s="40">
         <f t="shared" si="37"/>
         <v>99</v>
       </c>
-      <c r="I165" s="29"/>
+      <c r="I165" s="40"/>
       <c r="J165" s="32"/>
-      <c r="K165" s="28">
+      <c r="K165" s="38">
         <v>566.69000000000005</v>
       </c>
-      <c r="L165" s="28"/>
-      <c r="M165" s="29">
+      <c r="L165" s="38"/>
+      <c r="M165" s="40">
         <f>K165-273.15</f>
         <v>293.54000000000008</v>
       </c>
-      <c r="N165" s="29"/>
+      <c r="N165" s="40"/>
       <c r="O165" s="35"/>
       <c r="P165" s="36"/>
     </row>
@@ -5274,25 +5397,25 @@
       <c r="E166" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F166" s="28">
+      <c r="F166" s="38">
         <v>261.92</v>
       </c>
-      <c r="G166" s="28"/>
-      <c r="H166" s="29">
+      <c r="G166" s="38"/>
+      <c r="H166" s="40">
         <f t="shared" si="37"/>
         <v>-11.229999999999961</v>
       </c>
-      <c r="I166" s="29"/>
+      <c r="I166" s="40"/>
       <c r="J166" s="32"/>
-      <c r="K166" s="28">
+      <c r="K166" s="38">
         <v>270.13</v>
       </c>
-      <c r="L166" s="28"/>
-      <c r="M166" s="29">
+      <c r="L166" s="38"/>
+      <c r="M166" s="40">
         <f t="shared" ref="M166:M170" si="39">K166-273.15</f>
         <v>-3.0199999999999818</v>
       </c>
-      <c r="N166" s="29"/>
+      <c r="N166" s="40"/>
       <c r="O166" s="35"/>
       <c r="P166" s="36"/>
     </row>
@@ -5300,25 +5423,25 @@
       <c r="E167" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F167" s="28">
+      <c r="F167" s="38">
         <v>214.52</v>
       </c>
-      <c r="G167" s="28"/>
-      <c r="H167" s="29">
+      <c r="G167" s="38"/>
+      <c r="H167" s="40">
         <f t="shared" si="37"/>
         <v>-58.629999999999967</v>
       </c>
-      <c r="I167" s="29"/>
+      <c r="I167" s="40"/>
       <c r="J167" s="32"/>
-      <c r="K167" s="28">
+      <c r="K167" s="38">
         <v>243.61</v>
       </c>
-      <c r="L167" s="28"/>
-      <c r="M167" s="29">
+      <c r="L167" s="38"/>
+      <c r="M167" s="40">
         <f t="shared" si="39"/>
         <v>-29.539999999999964</v>
       </c>
-      <c r="N167" s="29"/>
+      <c r="N167" s="40"/>
       <c r="O167" s="35"/>
       <c r="P167" s="36"/>
     </row>
@@ -5326,25 +5449,25 @@
       <c r="E168" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F168" s="28">
+      <c r="F168" s="38">
         <v>261.92</v>
       </c>
-      <c r="G168" s="28"/>
-      <c r="H168" s="29">
+      <c r="G168" s="38"/>
+      <c r="H168" s="40">
         <f t="shared" si="37"/>
         <v>-11.229999999999961</v>
       </c>
-      <c r="I168" s="29"/>
+      <c r="I168" s="40"/>
       <c r="J168" s="32"/>
-      <c r="K168" s="28">
+      <c r="K168" s="38">
         <v>270.13</v>
       </c>
-      <c r="L168" s="28"/>
-      <c r="M168" s="29">
+      <c r="L168" s="38"/>
+      <c r="M168" s="40">
         <f t="shared" si="39"/>
         <v>-3.0199999999999818</v>
       </c>
-      <c r="N168" s="29"/>
+      <c r="N168" s="40"/>
       <c r="O168" s="35"/>
       <c r="P168" s="36"/>
     </row>
@@ -5352,25 +5475,25 @@
       <c r="E169" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F169" s="28">
+      <c r="F169" s="38">
         <v>214.52</v>
       </c>
-      <c r="G169" s="28"/>
-      <c r="H169" s="29">
+      <c r="G169" s="38"/>
+      <c r="H169" s="40">
         <f t="shared" si="37"/>
         <v>-58.629999999999967</v>
       </c>
-      <c r="I169" s="29"/>
+      <c r="I169" s="40"/>
       <c r="J169" s="32"/>
-      <c r="K169" s="28">
+      <c r="K169" s="38">
         <v>243.61</v>
       </c>
-      <c r="L169" s="28"/>
-      <c r="M169" s="29">
+      <c r="L169" s="38"/>
+      <c r="M169" s="40">
         <f t="shared" si="39"/>
         <v>-29.539999999999964</v>
       </c>
-      <c r="N169" s="29"/>
+      <c r="N169" s="40"/>
       <c r="O169" s="35"/>
       <c r="P169" s="36"/>
     </row>
@@ -5378,25 +5501,25 @@
       <c r="E170" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F170" s="28">
+      <c r="F170" s="38">
         <v>305.83999999999997</v>
       </c>
-      <c r="G170" s="28"/>
-      <c r="H170" s="29">
+      <c r="G170" s="38"/>
+      <c r="H170" s="40">
         <f t="shared" si="37"/>
         <v>32.69</v>
       </c>
-      <c r="I170" s="29"/>
+      <c r="I170" s="40"/>
       <c r="J170" s="32"/>
-      <c r="K170" s="28">
+      <c r="K170" s="38">
         <v>301.44</v>
       </c>
-      <c r="L170" s="28"/>
-      <c r="M170" s="29">
+      <c r="L170" s="38"/>
+      <c r="M170" s="40">
         <f t="shared" si="39"/>
         <v>28.29000000000002</v>
       </c>
-      <c r="N170" s="29"/>
+      <c r="N170" s="40"/>
       <c r="O170" s="35"/>
       <c r="P170" s="36"/>
     </row>
@@ -5409,10 +5532,10 @@
       </c>
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="F173" s="27" t="s">
+      <c r="F173" s="30" t="s">
         <v>75</v>
       </c>
-      <c r="G173" s="27"/>
+      <c r="G173" s="30"/>
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F174" s="15">
@@ -5497,6 +5620,123 @@
     </row>
   </sheetData>
   <mergeCells count="141">
+    <mergeCell ref="F173:G173"/>
+    <mergeCell ref="K167:L167"/>
+    <mergeCell ref="M167:N167"/>
+    <mergeCell ref="K168:L168"/>
+    <mergeCell ref="M168:N168"/>
+    <mergeCell ref="K169:L169"/>
+    <mergeCell ref="M169:N169"/>
+    <mergeCell ref="F170:G170"/>
+    <mergeCell ref="H170:I170"/>
+    <mergeCell ref="H167:I167"/>
+    <mergeCell ref="H168:I168"/>
+    <mergeCell ref="H169:I169"/>
+    <mergeCell ref="M166:N166"/>
+    <mergeCell ref="F156:I158"/>
+    <mergeCell ref="K156:N158"/>
+    <mergeCell ref="A159:C166"/>
+    <mergeCell ref="J159:J170"/>
+    <mergeCell ref="K161:L161"/>
+    <mergeCell ref="M161:N161"/>
+    <mergeCell ref="K162:L162"/>
+    <mergeCell ref="M162:N162"/>
+    <mergeCell ref="K163:L163"/>
+    <mergeCell ref="M163:N163"/>
+    <mergeCell ref="K170:L170"/>
+    <mergeCell ref="M170:N170"/>
+    <mergeCell ref="H164:I164"/>
+    <mergeCell ref="H165:I165"/>
+    <mergeCell ref="H166:I166"/>
+    <mergeCell ref="K164:L164"/>
+    <mergeCell ref="O159:P159"/>
+    <mergeCell ref="O160:P170"/>
+    <mergeCell ref="F161:G161"/>
+    <mergeCell ref="F162:G162"/>
+    <mergeCell ref="F163:G163"/>
+    <mergeCell ref="F164:G164"/>
+    <mergeCell ref="F165:G165"/>
+    <mergeCell ref="F166:G166"/>
+    <mergeCell ref="F160:I160"/>
+    <mergeCell ref="F159:G159"/>
+    <mergeCell ref="H159:I159"/>
+    <mergeCell ref="K159:L159"/>
+    <mergeCell ref="M159:N159"/>
+    <mergeCell ref="K160:N160"/>
+    <mergeCell ref="F167:G167"/>
+    <mergeCell ref="F168:G168"/>
+    <mergeCell ref="F169:G169"/>
+    <mergeCell ref="H161:I161"/>
+    <mergeCell ref="H162:I162"/>
+    <mergeCell ref="H163:I163"/>
+    <mergeCell ref="M164:N164"/>
+    <mergeCell ref="K165:L165"/>
+    <mergeCell ref="M165:N165"/>
+    <mergeCell ref="K166:L166"/>
+    <mergeCell ref="A142:C149"/>
+    <mergeCell ref="J142:J153"/>
+    <mergeCell ref="O142:P142"/>
+    <mergeCell ref="F143:G143"/>
+    <mergeCell ref="H143:I143"/>
+    <mergeCell ref="K143:L143"/>
+    <mergeCell ref="M143:N143"/>
+    <mergeCell ref="O143:P153"/>
+    <mergeCell ref="F139:I141"/>
+    <mergeCell ref="K139:N141"/>
+    <mergeCell ref="F123:I123"/>
+    <mergeCell ref="A124:C131"/>
+    <mergeCell ref="J124:J135"/>
+    <mergeCell ref="O124:P124"/>
+    <mergeCell ref="F125:G125"/>
+    <mergeCell ref="H125:I125"/>
+    <mergeCell ref="K125:L125"/>
+    <mergeCell ref="M125:N125"/>
+    <mergeCell ref="O125:P135"/>
+    <mergeCell ref="A105:C111"/>
+    <mergeCell ref="J105:J115"/>
+    <mergeCell ref="O105:P105"/>
+    <mergeCell ref="F106:G106"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="K106:L106"/>
+    <mergeCell ref="M106:N106"/>
+    <mergeCell ref="O106:P115"/>
+    <mergeCell ref="F104:N104"/>
+    <mergeCell ref="F88:I88"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="A89:C95"/>
+    <mergeCell ref="J89:J99"/>
+    <mergeCell ref="O89:P89"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="K90:L90"/>
+    <mergeCell ref="M90:N90"/>
+    <mergeCell ref="O90:P99"/>
+    <mergeCell ref="O54:P54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="M55:N55"/>
+    <mergeCell ref="O55:P64"/>
+    <mergeCell ref="F70:I70"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="A71:C77"/>
+    <mergeCell ref="J71:J81"/>
+    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="H72:I72"/>
+    <mergeCell ref="K72:L72"/>
+    <mergeCell ref="M72:N72"/>
+    <mergeCell ref="O72:P81"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="J5:J15"/>
+    <mergeCell ref="F20:I20"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="A54:C60"/>
+    <mergeCell ref="J54:J64"/>
     <mergeCell ref="F4:I4"/>
     <mergeCell ref="K4:N4"/>
     <mergeCell ref="F6:G6"/>
@@ -5521,123 +5761,6 @@
     <mergeCell ref="O22:P31"/>
     <mergeCell ref="J21:J31"/>
     <mergeCell ref="K22:L22"/>
-    <mergeCell ref="M22:N22"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="J5:J15"/>
-    <mergeCell ref="F20:I20"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="A54:C60"/>
-    <mergeCell ref="J54:J64"/>
-    <mergeCell ref="O54:P54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="M55:N55"/>
-    <mergeCell ref="O55:P64"/>
-    <mergeCell ref="F70:I70"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="A71:C77"/>
-    <mergeCell ref="J71:J81"/>
-    <mergeCell ref="O71:P71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="H72:I72"/>
-    <mergeCell ref="K72:L72"/>
-    <mergeCell ref="M72:N72"/>
-    <mergeCell ref="O72:P81"/>
-    <mergeCell ref="F88:I88"/>
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="A89:C95"/>
-    <mergeCell ref="J89:J99"/>
-    <mergeCell ref="O89:P89"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="K90:L90"/>
-    <mergeCell ref="M90:N90"/>
-    <mergeCell ref="O90:P99"/>
-    <mergeCell ref="A105:C111"/>
-    <mergeCell ref="J105:J115"/>
-    <mergeCell ref="O105:P105"/>
-    <mergeCell ref="F106:G106"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="K106:L106"/>
-    <mergeCell ref="M106:N106"/>
-    <mergeCell ref="O106:P115"/>
-    <mergeCell ref="F104:N104"/>
-    <mergeCell ref="F123:I123"/>
-    <mergeCell ref="A124:C131"/>
-    <mergeCell ref="J124:J135"/>
-    <mergeCell ref="O124:P124"/>
-    <mergeCell ref="F125:G125"/>
-    <mergeCell ref="H125:I125"/>
-    <mergeCell ref="K125:L125"/>
-    <mergeCell ref="M125:N125"/>
-    <mergeCell ref="O125:P135"/>
-    <mergeCell ref="A142:C149"/>
-    <mergeCell ref="J142:J153"/>
-    <mergeCell ref="O142:P142"/>
-    <mergeCell ref="F143:G143"/>
-    <mergeCell ref="H143:I143"/>
-    <mergeCell ref="K143:L143"/>
-    <mergeCell ref="M143:N143"/>
-    <mergeCell ref="O143:P153"/>
-    <mergeCell ref="F139:I141"/>
-    <mergeCell ref="K139:N141"/>
-    <mergeCell ref="O159:P159"/>
-    <mergeCell ref="O160:P170"/>
-    <mergeCell ref="F161:G161"/>
-    <mergeCell ref="F162:G162"/>
-    <mergeCell ref="F163:G163"/>
-    <mergeCell ref="F164:G164"/>
-    <mergeCell ref="F165:G165"/>
-    <mergeCell ref="F166:G166"/>
-    <mergeCell ref="F160:I160"/>
-    <mergeCell ref="F159:G159"/>
-    <mergeCell ref="H159:I159"/>
-    <mergeCell ref="K159:L159"/>
-    <mergeCell ref="M159:N159"/>
-    <mergeCell ref="K160:N160"/>
-    <mergeCell ref="F167:G167"/>
-    <mergeCell ref="F168:G168"/>
-    <mergeCell ref="F169:G169"/>
-    <mergeCell ref="H161:I161"/>
-    <mergeCell ref="H162:I162"/>
-    <mergeCell ref="H163:I163"/>
-    <mergeCell ref="M164:N164"/>
-    <mergeCell ref="K165:L165"/>
-    <mergeCell ref="M165:N165"/>
-    <mergeCell ref="K166:L166"/>
-    <mergeCell ref="M166:N166"/>
-    <mergeCell ref="F156:I158"/>
-    <mergeCell ref="K156:N158"/>
-    <mergeCell ref="A159:C166"/>
-    <mergeCell ref="J159:J170"/>
-    <mergeCell ref="K161:L161"/>
-    <mergeCell ref="M161:N161"/>
-    <mergeCell ref="K162:L162"/>
-    <mergeCell ref="M162:N162"/>
-    <mergeCell ref="K163:L163"/>
-    <mergeCell ref="M163:N163"/>
-    <mergeCell ref="K170:L170"/>
-    <mergeCell ref="M170:N170"/>
-    <mergeCell ref="H164:I164"/>
-    <mergeCell ref="H165:I165"/>
-    <mergeCell ref="H166:I166"/>
-    <mergeCell ref="K164:L164"/>
-    <mergeCell ref="F173:G173"/>
-    <mergeCell ref="K167:L167"/>
-    <mergeCell ref="M167:N167"/>
-    <mergeCell ref="K168:L168"/>
-    <mergeCell ref="M168:N168"/>
-    <mergeCell ref="K169:L169"/>
-    <mergeCell ref="M169:N169"/>
-    <mergeCell ref="F170:G170"/>
-    <mergeCell ref="H170:I170"/>
-    <mergeCell ref="H167:I167"/>
-    <mergeCell ref="H168:I168"/>
-    <mergeCell ref="H169:I169"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5645,6 +5768,2772 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:L143"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="N125" sqref="N125"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="96.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="21.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E4" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E5" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="44"/>
+      <c r="G8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="34"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="E9" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="45"/>
+      <c r="G9" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30">
+        <v>0.75</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9" s="51"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="E10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="45"/>
+      <c r="G10" s="47">
+        <v>324.61</v>
+      </c>
+      <c r="H10" s="48">
+        <f>G10-273.15</f>
+        <v>51.460000000000036</v>
+      </c>
+      <c r="I10" s="47">
+        <v>315.92</v>
+      </c>
+      <c r="J10" s="48">
+        <f>I10-273.15</f>
+        <v>42.770000000000039</v>
+      </c>
+      <c r="K10" s="50"/>
+      <c r="L10" s="51"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="E11" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F11" s="45"/>
+      <c r="G11" s="47">
+        <v>324.62</v>
+      </c>
+      <c r="H11" s="48">
+        <f t="shared" ref="H11:H29" si="0">G11-273.15</f>
+        <v>51.470000000000027</v>
+      </c>
+      <c r="I11" s="47">
+        <v>315.94</v>
+      </c>
+      <c r="J11" s="48">
+        <f t="shared" ref="J11:J29" si="1">I11-273.15</f>
+        <v>42.79000000000002</v>
+      </c>
+      <c r="K11" s="50"/>
+      <c r="L11" s="51"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="E12" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="45"/>
+      <c r="G12" s="47">
+        <v>324.44</v>
+      </c>
+      <c r="H12" s="48">
+        <f t="shared" si="0"/>
+        <v>51.29000000000002</v>
+      </c>
+      <c r="I12" s="47">
+        <v>315.77</v>
+      </c>
+      <c r="J12" s="48">
+        <f t="shared" si="1"/>
+        <v>42.620000000000005</v>
+      </c>
+      <c r="K12" s="50"/>
+      <c r="L12" s="51"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="31"/>
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="E13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="45"/>
+      <c r="G13" s="47">
+        <v>324.44</v>
+      </c>
+      <c r="H13" s="48">
+        <f t="shared" si="0"/>
+        <v>51.29000000000002</v>
+      </c>
+      <c r="I13" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="J13" s="48">
+        <f t="shared" si="1"/>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="K13" s="50"/>
+      <c r="L13" s="51"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="31"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="E14" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="45"/>
+      <c r="G14" s="47">
+        <v>324.43</v>
+      </c>
+      <c r="H14" s="48">
+        <f t="shared" si="0"/>
+        <v>51.28000000000003</v>
+      </c>
+      <c r="I14" s="47">
+        <v>315.77</v>
+      </c>
+      <c r="J14" s="48">
+        <f t="shared" si="1"/>
+        <v>42.620000000000005</v>
+      </c>
+      <c r="K14" s="50"/>
+      <c r="L14" s="51"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="45"/>
+      <c r="G15" s="47">
+        <v>324.43</v>
+      </c>
+      <c r="H15" s="48">
+        <f t="shared" si="0"/>
+        <v>51.28000000000003</v>
+      </c>
+      <c r="I15" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="J15" s="48">
+        <f t="shared" si="1"/>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="K15" s="50"/>
+      <c r="L15" s="51"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="45"/>
+      <c r="G16" s="47">
+        <v>413.74</v>
+      </c>
+      <c r="H16" s="48">
+        <f t="shared" si="0"/>
+        <v>140.59000000000003</v>
+      </c>
+      <c r="I16" s="47">
+        <v>396.7</v>
+      </c>
+      <c r="J16" s="48">
+        <f t="shared" si="1"/>
+        <v>123.55000000000001</v>
+      </c>
+      <c r="K16" s="50"/>
+      <c r="L16" s="51"/>
+    </row>
+    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="G17" s="47">
+        <v>404.01</v>
+      </c>
+      <c r="H17" s="48">
+        <f t="shared" si="0"/>
+        <v>130.86000000000001</v>
+      </c>
+      <c r="I17" s="47">
+        <v>386.1</v>
+      </c>
+      <c r="J17" s="48">
+        <f t="shared" si="1"/>
+        <v>112.95000000000005</v>
+      </c>
+      <c r="K17" s="50"/>
+      <c r="L17" s="51"/>
+    </row>
+    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="45"/>
+      <c r="G18" s="47">
+        <v>310.52999999999997</v>
+      </c>
+      <c r="H18" s="48">
+        <f t="shared" si="0"/>
+        <v>37.379999999999995</v>
+      </c>
+      <c r="I18" s="47">
+        <v>310.02999999999997</v>
+      </c>
+      <c r="J18" s="48">
+        <f t="shared" si="1"/>
+        <v>36.879999999999995</v>
+      </c>
+      <c r="K18" s="50"/>
+      <c r="L18" s="51"/>
+    </row>
+    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="45"/>
+      <c r="G19" s="49">
+        <v>309.11</v>
+      </c>
+      <c r="H19" s="48">
+        <f t="shared" si="0"/>
+        <v>35.960000000000036</v>
+      </c>
+      <c r="I19" s="49">
+        <v>308.86</v>
+      </c>
+      <c r="J19" s="48">
+        <f t="shared" si="1"/>
+        <v>35.710000000000036</v>
+      </c>
+      <c r="K19" s="50"/>
+      <c r="L19" s="51"/>
+    </row>
+    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="45"/>
+      <c r="G20" s="49">
+        <v>309.08999999999997</v>
+      </c>
+      <c r="H20" s="48">
+        <f t="shared" si="0"/>
+        <v>35.94</v>
+      </c>
+      <c r="I20" s="49">
+        <v>308.83999999999997</v>
+      </c>
+      <c r="J20" s="48">
+        <f t="shared" si="1"/>
+        <v>35.69</v>
+      </c>
+      <c r="K20" s="50"/>
+      <c r="L20" s="51"/>
+    </row>
+    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="45"/>
+      <c r="G21" s="47">
+        <v>308.99</v>
+      </c>
+      <c r="H21" s="48">
+        <f t="shared" si="0"/>
+        <v>35.840000000000032</v>
+      </c>
+      <c r="I21" s="47">
+        <v>308.8</v>
+      </c>
+      <c r="J21" s="48">
+        <f t="shared" si="1"/>
+        <v>35.650000000000034</v>
+      </c>
+      <c r="K21" s="50"/>
+      <c r="L21" s="51"/>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E22" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F22" s="45"/>
+      <c r="G22" s="47">
+        <v>324.43</v>
+      </c>
+      <c r="H22" s="48">
+        <f t="shared" si="0"/>
+        <v>51.28000000000003</v>
+      </c>
+      <c r="I22" s="47">
+        <v>315.66000000000003</v>
+      </c>
+      <c r="J22" s="48">
+        <f t="shared" si="1"/>
+        <v>42.510000000000048</v>
+      </c>
+      <c r="K22" s="50"/>
+      <c r="L22" s="51"/>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E23" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F23" s="45"/>
+      <c r="G23" s="47">
+        <v>324.49</v>
+      </c>
+      <c r="H23" s="48">
+        <f t="shared" si="0"/>
+        <v>51.340000000000032</v>
+      </c>
+      <c r="I23" s="47">
+        <v>315.83</v>
+      </c>
+      <c r="J23" s="48">
+        <f t="shared" si="1"/>
+        <v>42.680000000000007</v>
+      </c>
+      <c r="K23" s="50"/>
+      <c r="L23" s="51"/>
+    </row>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E24" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F24" s="45"/>
+      <c r="G24" s="47">
+        <v>324.44</v>
+      </c>
+      <c r="H24" s="48">
+        <f t="shared" si="0"/>
+        <v>51.29000000000002</v>
+      </c>
+      <c r="I24" s="47">
+        <v>315.7</v>
+      </c>
+      <c r="J24" s="48">
+        <f t="shared" si="1"/>
+        <v>42.550000000000011</v>
+      </c>
+      <c r="K24" s="50"/>
+      <c r="L24" s="51"/>
+    </row>
+    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="45"/>
+      <c r="G25" s="47">
+        <v>308.43</v>
+      </c>
+      <c r="H25" s="48">
+        <f t="shared" si="0"/>
+        <v>35.28000000000003</v>
+      </c>
+      <c r="I25" s="47">
+        <v>308.24</v>
+      </c>
+      <c r="J25" s="48">
+        <f t="shared" si="1"/>
+        <v>35.090000000000032</v>
+      </c>
+      <c r="K25" s="50"/>
+      <c r="L25" s="51"/>
+    </row>
+    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="45"/>
+      <c r="G26" s="47">
+        <v>308.38</v>
+      </c>
+      <c r="H26" s="48">
+        <f t="shared" si="0"/>
+        <v>35.230000000000018</v>
+      </c>
+      <c r="I26" s="47">
+        <v>308.19</v>
+      </c>
+      <c r="J26" s="48">
+        <f t="shared" si="1"/>
+        <v>35.04000000000002</v>
+      </c>
+      <c r="K26" s="50"/>
+      <c r="L26" s="51"/>
+    </row>
+    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E27" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="45"/>
+      <c r="G27" s="47">
+        <v>308.77</v>
+      </c>
+      <c r="H27" s="48">
+        <f t="shared" si="0"/>
+        <v>35.620000000000005</v>
+      </c>
+      <c r="I27" s="47">
+        <v>308.95999999999998</v>
+      </c>
+      <c r="J27" s="48">
+        <f t="shared" si="1"/>
+        <v>35.81</v>
+      </c>
+      <c r="K27" s="50"/>
+      <c r="L27" s="51"/>
+    </row>
+    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E28" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" s="45"/>
+      <c r="G28" s="47">
+        <v>308.72000000000003</v>
+      </c>
+      <c r="H28" s="48">
+        <f t="shared" si="0"/>
+        <v>35.57000000000005</v>
+      </c>
+      <c r="I28" s="47">
+        <v>308.89999999999998</v>
+      </c>
+      <c r="J28" s="48">
+        <f t="shared" si="1"/>
+        <v>35.75</v>
+      </c>
+      <c r="K28" s="50"/>
+      <c r="L28" s="51"/>
+    </row>
+    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="46"/>
+      <c r="G29" s="47">
+        <v>323.55</v>
+      </c>
+      <c r="H29" s="48">
+        <f t="shared" si="0"/>
+        <v>50.400000000000034</v>
+      </c>
+      <c r="I29" s="47">
+        <v>317.95999999999998</v>
+      </c>
+      <c r="J29" s="48">
+        <f t="shared" si="1"/>
+        <v>44.81</v>
+      </c>
+      <c r="K29" s="50"/>
+      <c r="L29" s="51"/>
+    </row>
+    <row r="32" spans="5:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E32" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E33" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E35" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="E36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="44"/>
+      <c r="G36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K36" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L36" s="34"/>
+    </row>
+    <row r="37" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="E37" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" s="45"/>
+      <c r="G37" s="30">
+        <v>1E-3</v>
+      </c>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30">
+        <v>400</v>
+      </c>
+      <c r="J37" s="30"/>
+      <c r="K37" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="L37" s="51"/>
+    </row>
+    <row r="38" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="E38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F38" s="45"/>
+      <c r="G38" s="47">
+        <v>367.57</v>
+      </c>
+      <c r="H38" s="48">
+        <f>G38-273.15</f>
+        <v>94.420000000000016</v>
+      </c>
+      <c r="I38" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="J38" s="48">
+        <f>I38-273.15</f>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="K38" s="50"/>
+      <c r="L38" s="51"/>
+    </row>
+    <row r="39" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="E39" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F39" s="45"/>
+      <c r="G39" s="47">
+        <v>367.71</v>
+      </c>
+      <c r="H39" s="48">
+        <f t="shared" ref="H39:H57" si="2">G39-273.15</f>
+        <v>94.56</v>
+      </c>
+      <c r="I39" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="J39" s="48">
+        <f t="shared" ref="J39:J57" si="3">I39-273.15</f>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="K39" s="50"/>
+      <c r="L39" s="51"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="E40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="45"/>
+      <c r="G40" s="47">
+        <v>367.36</v>
+      </c>
+      <c r="H40" s="48">
+        <f t="shared" si="2"/>
+        <v>94.210000000000036</v>
+      </c>
+      <c r="I40" s="47">
+        <v>315.64</v>
+      </c>
+      <c r="J40" s="48">
+        <f t="shared" si="3"/>
+        <v>42.490000000000009</v>
+      </c>
+      <c r="K40" s="50"/>
+      <c r="L40" s="51"/>
+    </row>
+    <row r="41" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="31"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="E41" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F41" s="45"/>
+      <c r="G41" s="47">
+        <v>367.51</v>
+      </c>
+      <c r="H41" s="48">
+        <f t="shared" si="2"/>
+        <v>94.360000000000014</v>
+      </c>
+      <c r="I41" s="47">
+        <v>315.64</v>
+      </c>
+      <c r="J41" s="48">
+        <f t="shared" si="3"/>
+        <v>42.490000000000009</v>
+      </c>
+      <c r="K41" s="50"/>
+      <c r="L41" s="51"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="31"/>
+      <c r="E42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="45"/>
+      <c r="G42" s="47">
+        <v>367.35</v>
+      </c>
+      <c r="H42" s="48">
+        <f t="shared" si="2"/>
+        <v>94.200000000000045</v>
+      </c>
+      <c r="I42" s="47">
+        <v>315.64</v>
+      </c>
+      <c r="J42" s="48">
+        <f t="shared" si="3"/>
+        <v>42.490000000000009</v>
+      </c>
+      <c r="K42" s="50"/>
+      <c r="L42" s="51"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E43" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="45"/>
+      <c r="G43" s="47">
+        <v>367.5</v>
+      </c>
+      <c r="H43" s="48">
+        <f t="shared" si="2"/>
+        <v>94.350000000000023</v>
+      </c>
+      <c r="I43" s="47">
+        <v>315.64</v>
+      </c>
+      <c r="J43" s="48">
+        <f t="shared" si="3"/>
+        <v>42.490000000000009</v>
+      </c>
+      <c r="K43" s="50"/>
+      <c r="L43" s="51"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="45"/>
+      <c r="G44" s="47">
+        <v>437.69</v>
+      </c>
+      <c r="H44" s="48">
+        <f t="shared" si="2"/>
+        <v>164.54000000000002</v>
+      </c>
+      <c r="I44" s="47">
+        <v>396.42</v>
+      </c>
+      <c r="J44" s="48">
+        <f t="shared" si="3"/>
+        <v>123.27000000000004</v>
+      </c>
+      <c r="K44" s="50"/>
+      <c r="L44" s="51"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E45" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F45" s="45"/>
+      <c r="G45" s="47">
+        <v>427.62</v>
+      </c>
+      <c r="H45" s="48">
+        <f t="shared" si="2"/>
+        <v>154.47000000000003</v>
+      </c>
+      <c r="I45" s="47">
+        <v>385.81</v>
+      </c>
+      <c r="J45" s="48">
+        <f t="shared" si="3"/>
+        <v>112.66000000000003</v>
+      </c>
+      <c r="K45" s="50"/>
+      <c r="L45" s="51"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E46" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F46" s="45"/>
+      <c r="G46" s="47">
+        <v>387.3</v>
+      </c>
+      <c r="H46" s="48">
+        <f t="shared" si="2"/>
+        <v>114.15000000000003</v>
+      </c>
+      <c r="I46" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J46" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K46" s="50"/>
+      <c r="L46" s="51"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E47" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F47" s="45"/>
+      <c r="G47" s="49">
+        <v>374.78</v>
+      </c>
+      <c r="H47" s="48">
+        <f t="shared" si="2"/>
+        <v>101.63</v>
+      </c>
+      <c r="I47" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J47" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K47" s="50"/>
+      <c r="L47" s="51"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E48" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F48" s="45"/>
+      <c r="G48" s="49">
+        <v>370.62</v>
+      </c>
+      <c r="H48" s="48">
+        <f t="shared" si="2"/>
+        <v>97.470000000000027</v>
+      </c>
+      <c r="I48" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J48" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K48" s="50"/>
+      <c r="L48" s="51"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="45"/>
+      <c r="G49" s="47">
+        <v>369.61</v>
+      </c>
+      <c r="H49" s="48">
+        <f t="shared" si="2"/>
+        <v>96.460000000000036</v>
+      </c>
+      <c r="I49" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J49" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K49" s="50"/>
+      <c r="L49" s="51"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E50" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F50" s="45"/>
+      <c r="G50" s="47">
+        <v>367.14</v>
+      </c>
+      <c r="H50" s="48">
+        <f t="shared" si="2"/>
+        <v>93.990000000000009</v>
+      </c>
+      <c r="I50" s="47">
+        <v>315.54000000000002</v>
+      </c>
+      <c r="J50" s="48">
+        <f t="shared" si="3"/>
+        <v>42.390000000000043</v>
+      </c>
+      <c r="K50" s="50"/>
+      <c r="L50" s="51"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E51" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" s="45"/>
+      <c r="G51" s="47">
+        <v>367.51</v>
+      </c>
+      <c r="H51" s="48">
+        <f t="shared" si="2"/>
+        <v>94.360000000000014</v>
+      </c>
+      <c r="I51" s="47">
+        <v>315.69</v>
+      </c>
+      <c r="J51" s="48">
+        <f t="shared" si="3"/>
+        <v>42.54000000000002</v>
+      </c>
+      <c r="K51" s="50"/>
+      <c r="L51" s="51"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F52" s="45"/>
+      <c r="G52" s="47">
+        <v>367.4</v>
+      </c>
+      <c r="H52" s="48">
+        <f t="shared" si="2"/>
+        <v>94.25</v>
+      </c>
+      <c r="I52" s="47">
+        <v>315.54000000000002</v>
+      </c>
+      <c r="J52" s="48">
+        <f t="shared" si="3"/>
+        <v>42.390000000000043</v>
+      </c>
+      <c r="K52" s="50"/>
+      <c r="L52" s="51"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="45"/>
+      <c r="G53" s="47">
+        <v>358.88</v>
+      </c>
+      <c r="H53" s="48">
+        <f t="shared" si="2"/>
+        <v>85.730000000000018</v>
+      </c>
+      <c r="I53" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J53" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K53" s="50"/>
+      <c r="L53" s="51"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E54" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F54" s="45"/>
+      <c r="G54" s="47">
+        <v>308.17</v>
+      </c>
+      <c r="H54" s="48">
+        <f t="shared" si="2"/>
+        <v>35.020000000000039</v>
+      </c>
+      <c r="I54" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J54" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K54" s="50"/>
+      <c r="L54" s="51"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F55" s="45"/>
+      <c r="G55" s="47">
+        <v>362.09</v>
+      </c>
+      <c r="H55" s="48">
+        <f t="shared" si="2"/>
+        <v>88.94</v>
+      </c>
+      <c r="I55" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J55" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K55" s="50"/>
+      <c r="L55" s="51"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E56" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" s="45"/>
+      <c r="G56" s="47">
+        <v>308.93</v>
+      </c>
+      <c r="H56" s="48">
+        <f t="shared" si="2"/>
+        <v>35.78000000000003</v>
+      </c>
+      <c r="I56" s="47">
+        <v>308.55</v>
+      </c>
+      <c r="J56" s="48">
+        <f t="shared" si="3"/>
+        <v>35.400000000000034</v>
+      </c>
+      <c r="K56" s="50"/>
+      <c r="L56" s="51"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E57" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F57" s="46"/>
+      <c r="G57" s="47">
+        <v>370.51</v>
+      </c>
+      <c r="H57" s="48">
+        <f t="shared" si="2"/>
+        <v>97.360000000000014</v>
+      </c>
+      <c r="I57" s="47">
+        <v>317.77</v>
+      </c>
+      <c r="J57" s="48">
+        <f t="shared" si="3"/>
+        <v>44.620000000000005</v>
+      </c>
+      <c r="K57" s="50"/>
+      <c r="L57" s="51"/>
+    </row>
+    <row r="60" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E60" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E61" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E62" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+    </row>
+    <row r="63" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E63" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F63" s="10"/>
+      <c r="G63" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="29"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+    </row>
+    <row r="64" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="31"/>
+      <c r="C64" s="31"/>
+      <c r="E64" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="44"/>
+      <c r="G64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K64" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L64" s="34"/>
+    </row>
+    <row r="65" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="31"/>
+      <c r="B65" s="31"/>
+      <c r="C65" s="31"/>
+      <c r="E65" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F65" s="45"/>
+      <c r="G65" s="30">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H65" s="30"/>
+      <c r="I65" s="30">
+        <v>0.05</v>
+      </c>
+      <c r="J65" s="30"/>
+      <c r="K65" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="L65" s="51"/>
+    </row>
+    <row r="66" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="31"/>
+      <c r="B66" s="31"/>
+      <c r="C66" s="31"/>
+      <c r="E66" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F66" s="45"/>
+      <c r="G66" s="47">
+        <v>315.92</v>
+      </c>
+      <c r="H66" s="48">
+        <f>G66-273.15</f>
+        <v>42.770000000000039</v>
+      </c>
+      <c r="I66" s="47">
+        <v>322.91000000000003</v>
+      </c>
+      <c r="J66" s="48">
+        <f>I66-273.15</f>
+        <v>49.760000000000048</v>
+      </c>
+      <c r="K66" s="50"/>
+      <c r="L66" s="51"/>
+    </row>
+    <row r="67" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="31"/>
+      <c r="B67" s="31"/>
+      <c r="C67" s="31"/>
+      <c r="E67" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F67" s="45"/>
+      <c r="G67" s="47">
+        <v>315.94</v>
+      </c>
+      <c r="H67" s="48">
+        <f t="shared" ref="H67:H85" si="4">G67-273.15</f>
+        <v>42.79000000000002</v>
+      </c>
+      <c r="I67" s="47">
+        <v>323</v>
+      </c>
+      <c r="J67" s="48">
+        <f t="shared" ref="J67:J85" si="5">I67-273.15</f>
+        <v>49.850000000000023</v>
+      </c>
+      <c r="K67" s="50"/>
+      <c r="L67" s="51"/>
+    </row>
+    <row r="68" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="31"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
+      <c r="E68" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F68" s="45"/>
+      <c r="G68" s="47">
+        <v>315.77</v>
+      </c>
+      <c r="H68" s="48">
+        <f t="shared" si="4"/>
+        <v>42.620000000000005</v>
+      </c>
+      <c r="I68" s="47">
+        <v>322.74</v>
+      </c>
+      <c r="J68" s="48">
+        <f t="shared" si="5"/>
+        <v>49.590000000000032</v>
+      </c>
+      <c r="K68" s="50"/>
+      <c r="L68" s="51"/>
+    </row>
+    <row r="69" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="31"/>
+      <c r="E69" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F69" s="45"/>
+      <c r="G69" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="H69" s="48">
+        <f t="shared" si="4"/>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="I69" s="47">
+        <v>322.83</v>
+      </c>
+      <c r="J69" s="48">
+        <f t="shared" si="5"/>
+        <v>49.680000000000007</v>
+      </c>
+      <c r="K69" s="50"/>
+      <c r="L69" s="51"/>
+    </row>
+    <row r="70" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="31"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="31"/>
+      <c r="E70" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F70" s="45"/>
+      <c r="G70" s="47">
+        <v>315.77</v>
+      </c>
+      <c r="H70" s="48">
+        <f t="shared" si="4"/>
+        <v>42.620000000000005</v>
+      </c>
+      <c r="I70" s="47">
+        <v>322.73</v>
+      </c>
+      <c r="J70" s="48">
+        <f t="shared" si="5"/>
+        <v>49.580000000000041</v>
+      </c>
+      <c r="K70" s="50"/>
+      <c r="L70" s="51"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E71" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F71" s="45"/>
+      <c r="G71" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="H71" s="48">
+        <f t="shared" si="4"/>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="I71" s="47">
+        <v>322.82</v>
+      </c>
+      <c r="J71" s="48">
+        <f t="shared" si="5"/>
+        <v>49.670000000000016</v>
+      </c>
+      <c r="K71" s="50"/>
+      <c r="L71" s="51"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E72" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F72" s="45"/>
+      <c r="G72" s="47">
+        <v>396.7</v>
+      </c>
+      <c r="H72" s="48">
+        <f t="shared" si="4"/>
+        <v>123.55000000000001</v>
+      </c>
+      <c r="I72" s="47">
+        <v>404.38</v>
+      </c>
+      <c r="J72" s="48">
+        <f t="shared" si="5"/>
+        <v>131.23000000000002</v>
+      </c>
+      <c r="K72" s="50"/>
+      <c r="L72" s="51"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E73" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F73" s="45"/>
+      <c r="G73" s="47">
+        <v>386.1</v>
+      </c>
+      <c r="H73" s="48">
+        <f t="shared" si="4"/>
+        <v>112.95000000000005</v>
+      </c>
+      <c r="I73" s="47">
+        <v>393.86</v>
+      </c>
+      <c r="J73" s="48">
+        <f t="shared" si="5"/>
+        <v>120.71000000000004</v>
+      </c>
+      <c r="K73" s="50"/>
+      <c r="L73" s="51"/>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E74" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F74" s="45"/>
+      <c r="G74" s="47">
+        <v>310.02999999999997</v>
+      </c>
+      <c r="H74" s="48">
+        <f t="shared" si="4"/>
+        <v>36.879999999999995</v>
+      </c>
+      <c r="I74" s="47">
+        <v>341.22</v>
+      </c>
+      <c r="J74" s="48">
+        <f t="shared" si="5"/>
+        <v>68.07000000000005</v>
+      </c>
+      <c r="K74" s="50"/>
+      <c r="L74" s="51"/>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E75" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F75" s="45"/>
+      <c r="G75" s="49">
+        <v>308.86</v>
+      </c>
+      <c r="H75" s="48">
+        <f t="shared" si="4"/>
+        <v>35.710000000000036</v>
+      </c>
+      <c r="I75" s="47">
+        <v>326.58</v>
+      </c>
+      <c r="J75" s="48">
+        <f t="shared" si="5"/>
+        <v>53.430000000000007</v>
+      </c>
+      <c r="K75" s="50"/>
+      <c r="L75" s="51"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E76" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F76" s="45"/>
+      <c r="G76" s="49">
+        <v>308.83999999999997</v>
+      </c>
+      <c r="H76" s="48">
+        <f t="shared" si="4"/>
+        <v>35.69</v>
+      </c>
+      <c r="I76" s="47">
+        <v>322.62</v>
+      </c>
+      <c r="J76" s="48">
+        <f t="shared" si="5"/>
+        <v>49.470000000000027</v>
+      </c>
+      <c r="K76" s="50"/>
+      <c r="L76" s="51"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E77" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F77" s="45"/>
+      <c r="G77" s="47">
+        <v>308.8</v>
+      </c>
+      <c r="H77" s="48">
+        <f t="shared" si="4"/>
+        <v>35.650000000000034</v>
+      </c>
+      <c r="I77" s="47">
+        <v>321.63</v>
+      </c>
+      <c r="J77" s="48">
+        <f t="shared" si="5"/>
+        <v>48.480000000000018</v>
+      </c>
+      <c r="K77" s="50"/>
+      <c r="L77" s="51"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E78" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F78" s="45"/>
+      <c r="G78" s="47">
+        <v>315.66000000000003</v>
+      </c>
+      <c r="H78" s="48">
+        <f t="shared" si="4"/>
+        <v>42.510000000000048</v>
+      </c>
+      <c r="I78" s="47">
+        <v>322.56</v>
+      </c>
+      <c r="J78" s="48">
+        <f t="shared" si="5"/>
+        <v>49.410000000000025</v>
+      </c>
+      <c r="K78" s="50"/>
+      <c r="L78" s="51"/>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E79" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F79" s="45"/>
+      <c r="G79" s="47">
+        <v>315.83</v>
+      </c>
+      <c r="H79" s="48">
+        <f t="shared" si="4"/>
+        <v>42.680000000000007</v>
+      </c>
+      <c r="I79" s="47">
+        <v>322.85000000000002</v>
+      </c>
+      <c r="J79" s="48">
+        <f t="shared" si="5"/>
+        <v>49.700000000000045</v>
+      </c>
+      <c r="K79" s="50"/>
+      <c r="L79" s="51"/>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E80" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F80" s="45"/>
+      <c r="G80" s="47">
+        <v>315.7</v>
+      </c>
+      <c r="H80" s="48">
+        <f t="shared" si="4"/>
+        <v>42.550000000000011</v>
+      </c>
+      <c r="I80" s="47">
+        <v>322.72000000000003</v>
+      </c>
+      <c r="J80" s="48">
+        <f t="shared" si="5"/>
+        <v>49.57000000000005</v>
+      </c>
+      <c r="K80" s="50"/>
+      <c r="L80" s="51"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E81" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" s="45"/>
+      <c r="G81" s="47">
+        <v>308.24</v>
+      </c>
+      <c r="H81" s="48">
+        <f t="shared" si="4"/>
+        <v>35.090000000000032</v>
+      </c>
+      <c r="I81" s="47">
+        <v>312.27</v>
+      </c>
+      <c r="J81" s="48">
+        <f t="shared" si="5"/>
+        <v>39.120000000000005</v>
+      </c>
+      <c r="K81" s="50"/>
+      <c r="L81" s="51"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E82" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F82" s="45"/>
+      <c r="G82" s="47">
+        <v>308.19</v>
+      </c>
+      <c r="H82" s="48">
+        <f t="shared" si="4"/>
+        <v>35.04000000000002</v>
+      </c>
+      <c r="I82" s="47">
+        <v>307.44</v>
+      </c>
+      <c r="J82" s="48">
+        <f t="shared" si="5"/>
+        <v>34.29000000000002</v>
+      </c>
+      <c r="K82" s="50"/>
+      <c r="L82" s="51"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E83" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F83" s="45"/>
+      <c r="G83" s="47">
+        <v>308.95999999999998</v>
+      </c>
+      <c r="H83" s="48">
+        <f t="shared" si="4"/>
+        <v>35.81</v>
+      </c>
+      <c r="I83" s="47">
+        <v>315.2</v>
+      </c>
+      <c r="J83" s="48">
+        <f t="shared" si="5"/>
+        <v>42.050000000000011</v>
+      </c>
+      <c r="K83" s="50"/>
+      <c r="L83" s="51"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E84" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F84" s="45"/>
+      <c r="G84" s="47">
+        <v>308.89999999999998</v>
+      </c>
+      <c r="H84" s="48">
+        <f t="shared" si="4"/>
+        <v>35.75</v>
+      </c>
+      <c r="I84" s="47">
+        <v>309.64</v>
+      </c>
+      <c r="J84" s="48">
+        <f t="shared" si="5"/>
+        <v>36.490000000000009</v>
+      </c>
+      <c r="K84" s="50"/>
+      <c r="L84" s="51"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E85" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F85" s="46"/>
+      <c r="G85" s="47">
+        <v>317.95999999999998</v>
+      </c>
+      <c r="H85" s="48">
+        <f t="shared" si="4"/>
+        <v>44.81</v>
+      </c>
+      <c r="I85" s="47">
+        <v>325.74</v>
+      </c>
+      <c r="J85" s="48">
+        <f t="shared" si="5"/>
+        <v>52.590000000000032</v>
+      </c>
+      <c r="K85" s="50"/>
+      <c r="L85" s="51"/>
+    </row>
+    <row r="88" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E88" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E89" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E90" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E91" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="1"/>
+      <c r="I91" s="1"/>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+    </row>
+    <row r="92" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E92" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F92" s="10"/>
+      <c r="G92" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
+      <c r="J92" s="29"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+    </row>
+    <row r="93" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="B93" s="31"/>
+      <c r="C93" s="31"/>
+      <c r="E93" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="44"/>
+      <c r="G93" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K93" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L93" s="34"/>
+    </row>
+    <row r="94" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="31"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="31"/>
+      <c r="E94" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="F94" s="45"/>
+      <c r="G94" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H94" s="30"/>
+      <c r="I94" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="J94" s="30"/>
+      <c r="K94" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="L94" s="51"/>
+    </row>
+    <row r="95" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="31"/>
+      <c r="B95" s="31"/>
+      <c r="C95" s="31"/>
+      <c r="E95" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F95" s="45"/>
+      <c r="G95" s="47">
+        <v>315.92</v>
+      </c>
+      <c r="H95" s="48">
+        <f>G95-273.15</f>
+        <v>42.770000000000039</v>
+      </c>
+      <c r="I95" s="47">
+        <v>303.85000000000002</v>
+      </c>
+      <c r="J95" s="48">
+        <f>I95-273.15</f>
+        <v>30.700000000000045</v>
+      </c>
+      <c r="K95" s="50"/>
+      <c r="L95" s="51"/>
+    </row>
+    <row r="96" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="31"/>
+      <c r="B96" s="31"/>
+      <c r="C96" s="31"/>
+      <c r="E96" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F96" s="45"/>
+      <c r="G96" s="47">
+        <v>315.94</v>
+      </c>
+      <c r="H96" s="48">
+        <f t="shared" ref="H96:H114" si="6">G96-273.15</f>
+        <v>42.79000000000002</v>
+      </c>
+      <c r="I96" s="47">
+        <v>303.86</v>
+      </c>
+      <c r="J96" s="48">
+        <f t="shared" ref="J96:J114" si="7">I96-273.15</f>
+        <v>30.710000000000036</v>
+      </c>
+      <c r="K96" s="50"/>
+      <c r="L96" s="51"/>
+    </row>
+    <row r="97" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="31"/>
+      <c r="B97" s="31"/>
+      <c r="C97" s="31"/>
+      <c r="E97" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F97" s="45"/>
+      <c r="G97" s="47">
+        <v>315.77</v>
+      </c>
+      <c r="H97" s="48">
+        <f t="shared" si="6"/>
+        <v>42.620000000000005</v>
+      </c>
+      <c r="I97" s="47">
+        <v>303.70999999999998</v>
+      </c>
+      <c r="J97" s="48">
+        <f t="shared" si="7"/>
+        <v>30.560000000000002</v>
+      </c>
+      <c r="K97" s="50"/>
+      <c r="L97" s="51"/>
+    </row>
+    <row r="98" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A98" s="31"/>
+      <c r="B98" s="31"/>
+      <c r="C98" s="31"/>
+      <c r="E98" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F98" s="45"/>
+      <c r="G98" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="H98" s="48">
+        <f t="shared" si="6"/>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="I98" s="47">
+        <v>303.73</v>
+      </c>
+      <c r="J98" s="48">
+        <f t="shared" si="7"/>
+        <v>30.580000000000041</v>
+      </c>
+      <c r="K98" s="50"/>
+      <c r="L98" s="51"/>
+    </row>
+    <row r="99" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="31"/>
+      <c r="B99" s="31"/>
+      <c r="C99" s="31"/>
+      <c r="E99" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F99" s="45"/>
+      <c r="G99" s="47">
+        <v>315.77</v>
+      </c>
+      <c r="H99" s="48">
+        <f t="shared" si="6"/>
+        <v>42.620000000000005</v>
+      </c>
+      <c r="I99" s="47">
+        <v>303.70999999999998</v>
+      </c>
+      <c r="J99" s="48">
+        <f t="shared" si="7"/>
+        <v>30.560000000000002</v>
+      </c>
+      <c r="K99" s="50"/>
+      <c r="L99" s="51"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E100" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F100" s="45"/>
+      <c r="G100" s="47">
+        <v>315.79000000000002</v>
+      </c>
+      <c r="H100" s="48">
+        <f t="shared" si="6"/>
+        <v>42.640000000000043</v>
+      </c>
+      <c r="I100" s="47">
+        <v>303.73</v>
+      </c>
+      <c r="J100" s="48">
+        <f t="shared" si="7"/>
+        <v>30.580000000000041</v>
+      </c>
+      <c r="K100" s="50"/>
+      <c r="L100" s="51"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E101" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F101" s="45"/>
+      <c r="G101" s="47">
+        <v>396.7</v>
+      </c>
+      <c r="H101" s="48">
+        <f t="shared" si="6"/>
+        <v>123.55000000000001</v>
+      </c>
+      <c r="I101" s="47">
+        <v>386.15</v>
+      </c>
+      <c r="J101" s="48">
+        <f t="shared" si="7"/>
+        <v>113</v>
+      </c>
+      <c r="K101" s="50"/>
+      <c r="L101" s="51"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E102" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F102" s="45"/>
+      <c r="G102" s="47">
+        <v>386.1</v>
+      </c>
+      <c r="H102" s="48">
+        <f t="shared" si="6"/>
+        <v>112.95000000000005</v>
+      </c>
+      <c r="I102" s="47">
+        <v>375.66</v>
+      </c>
+      <c r="J102" s="48">
+        <f t="shared" si="7"/>
+        <v>102.51000000000005</v>
+      </c>
+      <c r="K102" s="50"/>
+      <c r="L102" s="51"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E103" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F103" s="45"/>
+      <c r="G103" s="47">
+        <v>310.02999999999997</v>
+      </c>
+      <c r="H103" s="48">
+        <f t="shared" si="6"/>
+        <v>36.879999999999995</v>
+      </c>
+      <c r="I103" s="47">
+        <v>297.2</v>
+      </c>
+      <c r="J103" s="48">
+        <f t="shared" si="7"/>
+        <v>24.050000000000011</v>
+      </c>
+      <c r="K103" s="50"/>
+      <c r="L103" s="51"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E104" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F104" s="45"/>
+      <c r="G104" s="49">
+        <v>308.86</v>
+      </c>
+      <c r="H104" s="48">
+        <f t="shared" si="6"/>
+        <v>35.710000000000036</v>
+      </c>
+      <c r="I104" s="47">
+        <v>296.02999999999997</v>
+      </c>
+      <c r="J104" s="48">
+        <f t="shared" si="7"/>
+        <v>22.879999999999995</v>
+      </c>
+      <c r="K104" s="50"/>
+      <c r="L104" s="51"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E105" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F105" s="45"/>
+      <c r="G105" s="49">
+        <v>308.83999999999997</v>
+      </c>
+      <c r="H105" s="48">
+        <f t="shared" si="6"/>
+        <v>35.69</v>
+      </c>
+      <c r="I105" s="47">
+        <v>296.02</v>
+      </c>
+      <c r="J105" s="48">
+        <f t="shared" si="7"/>
+        <v>22.870000000000005</v>
+      </c>
+      <c r="K105" s="50"/>
+      <c r="L105" s="51"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E106" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F106" s="45"/>
+      <c r="G106" s="47">
+        <v>308.8</v>
+      </c>
+      <c r="H106" s="48">
+        <f t="shared" si="6"/>
+        <v>35.650000000000034</v>
+      </c>
+      <c r="I106" s="47">
+        <v>295.98</v>
+      </c>
+      <c r="J106" s="48">
+        <f t="shared" si="7"/>
+        <v>22.830000000000041</v>
+      </c>
+      <c r="K106" s="50"/>
+      <c r="L106" s="51"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E107" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F107" s="45"/>
+      <c r="G107" s="47">
+        <v>315.66000000000003</v>
+      </c>
+      <c r="H107" s="48">
+        <f t="shared" si="6"/>
+        <v>42.510000000000048</v>
+      </c>
+      <c r="I107" s="47">
+        <v>303.60000000000002</v>
+      </c>
+      <c r="J107" s="48">
+        <f t="shared" si="7"/>
+        <v>30.450000000000045</v>
+      </c>
+      <c r="K107" s="50"/>
+      <c r="L107" s="51"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E108" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F108" s="45"/>
+      <c r="G108" s="47">
+        <v>315.83</v>
+      </c>
+      <c r="H108" s="48">
+        <f t="shared" si="6"/>
+        <v>42.680000000000007</v>
+      </c>
+      <c r="I108" s="47">
+        <v>303.77</v>
+      </c>
+      <c r="J108" s="48">
+        <f t="shared" si="7"/>
+        <v>30.620000000000005</v>
+      </c>
+      <c r="K108" s="50"/>
+      <c r="L108" s="51"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E109" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F109" s="45"/>
+      <c r="G109" s="47">
+        <v>315.7</v>
+      </c>
+      <c r="H109" s="48">
+        <f t="shared" si="6"/>
+        <v>42.550000000000011</v>
+      </c>
+      <c r="I109" s="47">
+        <v>303.63</v>
+      </c>
+      <c r="J109" s="48">
+        <f t="shared" si="7"/>
+        <v>30.480000000000018</v>
+      </c>
+      <c r="K109" s="50"/>
+      <c r="L109" s="51"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E110" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F110" s="45"/>
+      <c r="G110" s="47">
+        <v>308.24</v>
+      </c>
+      <c r="H110" s="48">
+        <f t="shared" si="6"/>
+        <v>35.090000000000032</v>
+      </c>
+      <c r="I110" s="47">
+        <v>295.44</v>
+      </c>
+      <c r="J110" s="48">
+        <f t="shared" si="7"/>
+        <v>22.29000000000002</v>
+      </c>
+      <c r="K110" s="50"/>
+      <c r="L110" s="51"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E111" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F111" s="45"/>
+      <c r="G111" s="47">
+        <v>308.19</v>
+      </c>
+      <c r="H111" s="48">
+        <f t="shared" si="6"/>
+        <v>35.04000000000002</v>
+      </c>
+      <c r="I111" s="47">
+        <v>295.39</v>
+      </c>
+      <c r="J111" s="48">
+        <f t="shared" si="7"/>
+        <v>22.240000000000009</v>
+      </c>
+      <c r="K111" s="50"/>
+      <c r="L111" s="51"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E112" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F112" s="45"/>
+      <c r="G112" s="47">
+        <v>308.95999999999998</v>
+      </c>
+      <c r="H112" s="48">
+        <f t="shared" si="6"/>
+        <v>35.81</v>
+      </c>
+      <c r="I112" s="47">
+        <v>296.06</v>
+      </c>
+      <c r="J112" s="48">
+        <f t="shared" si="7"/>
+        <v>22.910000000000025</v>
+      </c>
+      <c r="K112" s="50"/>
+      <c r="L112" s="51"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E113" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F113" s="45"/>
+      <c r="G113" s="47">
+        <v>308.89999999999998</v>
+      </c>
+      <c r="H113" s="48">
+        <f t="shared" si="6"/>
+        <v>35.75</v>
+      </c>
+      <c r="I113" s="47">
+        <v>296.01</v>
+      </c>
+      <c r="J113" s="48">
+        <f t="shared" si="7"/>
+        <v>22.860000000000014</v>
+      </c>
+      <c r="K113" s="50"/>
+      <c r="L113" s="51"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E114" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F114" s="46"/>
+      <c r="G114" s="47">
+        <v>317.95999999999998</v>
+      </c>
+      <c r="H114" s="48">
+        <f t="shared" si="6"/>
+        <v>44.81</v>
+      </c>
+      <c r="I114" s="47">
+        <v>305.94</v>
+      </c>
+      <c r="J114" s="48">
+        <f t="shared" si="7"/>
+        <v>32.79000000000002</v>
+      </c>
+      <c r="K114" s="50"/>
+      <c r="L114" s="51"/>
+    </row>
+    <row r="117" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E117" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E118" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E119" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E120" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="F120" s="1"/>
+      <c r="G120" s="1"/>
+      <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
+      <c r="J120" s="1"/>
+      <c r="K120" s="1"/>
+      <c r="L120" s="1"/>
+    </row>
+    <row r="121" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="E121" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F121" s="10"/>
+      <c r="G121" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="H121" s="29"/>
+      <c r="I121" s="29"/>
+      <c r="J121" s="29"/>
+      <c r="K121" s="1"/>
+      <c r="L121" s="1"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B122" s="31"/>
+      <c r="C122" s="31"/>
+      <c r="E122" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F122" s="44"/>
+      <c r="G122" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I122" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J122" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K122" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="L122" s="34"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" s="31"/>
+      <c r="B123" s="31"/>
+      <c r="C123" s="31"/>
+      <c r="E123" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="F123" s="45"/>
+      <c r="G123" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="H123" s="30"/>
+      <c r="I123" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="J123" s="30"/>
+      <c r="K123" s="50" t="s">
+        <v>129</v>
+      </c>
+      <c r="L123" s="51"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="31"/>
+      <c r="B124" s="31"/>
+      <c r="C124" s="31"/>
+      <c r="E124" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F124" s="45"/>
+      <c r="G124" s="47">
+        <v>657.35</v>
+      </c>
+      <c r="H124" s="48">
+        <f>G124-273.15</f>
+        <v>384.20000000000005</v>
+      </c>
+      <c r="I124" s="47">
+        <v>644.67999999999995</v>
+      </c>
+      <c r="J124" s="48">
+        <f>I124-273.15</f>
+        <v>371.53</v>
+      </c>
+      <c r="K124" s="50"/>
+      <c r="L124" s="51"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="31"/>
+      <c r="B125" s="31"/>
+      <c r="C125" s="31"/>
+      <c r="E125" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F125" s="45"/>
+      <c r="G125" s="47">
+        <v>657.58</v>
+      </c>
+      <c r="H125" s="48">
+        <f t="shared" ref="H125:H143" si="8">G125-273.15</f>
+        <v>384.43000000000006</v>
+      </c>
+      <c r="I125" s="47">
+        <v>644.91</v>
+      </c>
+      <c r="J125" s="48">
+        <f t="shared" ref="J125:J143" si="9">I125-273.15</f>
+        <v>371.76</v>
+      </c>
+      <c r="K125" s="50"/>
+      <c r="L125" s="51"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" s="31"/>
+      <c r="B126" s="31"/>
+      <c r="C126" s="31"/>
+      <c r="E126" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F126" s="45"/>
+      <c r="G126" s="47">
+        <v>657.04</v>
+      </c>
+      <c r="H126" s="48">
+        <f t="shared" si="8"/>
+        <v>383.89</v>
+      </c>
+      <c r="I126" s="47">
+        <v>644.37</v>
+      </c>
+      <c r="J126" s="48">
+        <f t="shared" si="9"/>
+        <v>371.22</v>
+      </c>
+      <c r="K126" s="50"/>
+      <c r="L126" s="51"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" s="31"/>
+      <c r="B127" s="31"/>
+      <c r="C127" s="31"/>
+      <c r="E127" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F127" s="45"/>
+      <c r="G127" s="47">
+        <v>657.27</v>
+      </c>
+      <c r="H127" s="48">
+        <f t="shared" si="8"/>
+        <v>384.12</v>
+      </c>
+      <c r="I127" s="47">
+        <v>644.6</v>
+      </c>
+      <c r="J127" s="48">
+        <f t="shared" si="9"/>
+        <v>371.45000000000005</v>
+      </c>
+      <c r="K127" s="50"/>
+      <c r="L127" s="51"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" s="31"/>
+      <c r="B128" s="31"/>
+      <c r="C128" s="31"/>
+      <c r="E128" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F128" s="45"/>
+      <c r="G128" s="47">
+        <v>657.02</v>
+      </c>
+      <c r="H128" s="48">
+        <f t="shared" si="8"/>
+        <v>383.87</v>
+      </c>
+      <c r="I128" s="47">
+        <v>644.34</v>
+      </c>
+      <c r="J128" s="48">
+        <f t="shared" si="9"/>
+        <v>371.19000000000005</v>
+      </c>
+      <c r="K128" s="50"/>
+      <c r="L128" s="51"/>
+    </row>
+    <row r="129" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E129" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F129" s="45"/>
+      <c r="G129" s="47">
+        <v>657.25</v>
+      </c>
+      <c r="H129" s="48">
+        <f t="shared" si="8"/>
+        <v>384.1</v>
+      </c>
+      <c r="I129" s="47">
+        <v>644.57000000000005</v>
+      </c>
+      <c r="J129" s="48">
+        <f t="shared" si="9"/>
+        <v>371.42000000000007</v>
+      </c>
+      <c r="K129" s="50"/>
+      <c r="L129" s="51"/>
+    </row>
+    <row r="130" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E130" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F130" s="45"/>
+      <c r="G130" s="47">
+        <v>682.88</v>
+      </c>
+      <c r="H130" s="48">
+        <f t="shared" si="8"/>
+        <v>409.73</v>
+      </c>
+      <c r="I130" s="47">
+        <v>671.34</v>
+      </c>
+      <c r="J130" s="48">
+        <f t="shared" si="9"/>
+        <v>398.19000000000005</v>
+      </c>
+      <c r="K130" s="50"/>
+      <c r="L130" s="51"/>
+    </row>
+    <row r="131" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E131" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F131" s="45"/>
+      <c r="G131" s="47">
+        <v>675.37</v>
+      </c>
+      <c r="H131" s="48">
+        <f t="shared" si="8"/>
+        <v>402.22</v>
+      </c>
+      <c r="I131" s="47">
+        <v>663.76</v>
+      </c>
+      <c r="J131" s="48">
+        <f t="shared" si="9"/>
+        <v>390.61</v>
+      </c>
+      <c r="K131" s="50"/>
+      <c r="L131" s="51"/>
+    </row>
+    <row r="132" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E132" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F132" s="45"/>
+      <c r="G132" s="47">
+        <v>663.56</v>
+      </c>
+      <c r="H132" s="48">
+        <f t="shared" si="8"/>
+        <v>390.40999999999997</v>
+      </c>
+      <c r="I132" s="47">
+        <v>651.20000000000005</v>
+      </c>
+      <c r="J132" s="48">
+        <f t="shared" si="9"/>
+        <v>378.05000000000007</v>
+      </c>
+      <c r="K132" s="50"/>
+      <c r="L132" s="51"/>
+    </row>
+    <row r="133" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E133" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F133" s="45"/>
+      <c r="G133" s="49">
+        <v>659.84</v>
+      </c>
+      <c r="H133" s="48">
+        <f t="shared" si="8"/>
+        <v>386.69000000000005</v>
+      </c>
+      <c r="I133" s="47">
+        <v>647.29</v>
+      </c>
+      <c r="J133" s="48">
+        <f t="shared" si="9"/>
+        <v>374.14</v>
+      </c>
+      <c r="K133" s="50"/>
+      <c r="L133" s="51"/>
+    </row>
+    <row r="134" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E134" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F134" s="45"/>
+      <c r="G134" s="49">
+        <v>658.38</v>
+      </c>
+      <c r="H134" s="48">
+        <f t="shared" si="8"/>
+        <v>385.23</v>
+      </c>
+      <c r="I134" s="47">
+        <v>645.77</v>
+      </c>
+      <c r="J134" s="48">
+        <f t="shared" si="9"/>
+        <v>372.62</v>
+      </c>
+      <c r="K134" s="50"/>
+      <c r="L134" s="51"/>
+    </row>
+    <row r="135" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E135" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F135" s="45"/>
+      <c r="G135" s="47">
+        <v>658.01</v>
+      </c>
+      <c r="H135" s="48">
+        <f t="shared" si="8"/>
+        <v>384.86</v>
+      </c>
+      <c r="I135" s="47">
+        <v>645.37</v>
+      </c>
+      <c r="J135" s="48">
+        <f t="shared" si="9"/>
+        <v>372.22</v>
+      </c>
+      <c r="K135" s="50"/>
+      <c r="L135" s="51"/>
+    </row>
+    <row r="136" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E136" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F136" s="45"/>
+      <c r="G136" s="47">
+        <v>656.86</v>
+      </c>
+      <c r="H136" s="48">
+        <f t="shared" si="8"/>
+        <v>383.71000000000004</v>
+      </c>
+      <c r="I136" s="47">
+        <v>644.19000000000005</v>
+      </c>
+      <c r="J136" s="48">
+        <f t="shared" si="9"/>
+        <v>371.04000000000008</v>
+      </c>
+      <c r="K136" s="50"/>
+      <c r="L136" s="51"/>
+    </row>
+    <row r="137" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E137" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F137" s="45"/>
+      <c r="G137" s="47">
+        <v>657.25</v>
+      </c>
+      <c r="H137" s="48">
+        <f t="shared" si="8"/>
+        <v>384.1</v>
+      </c>
+      <c r="I137" s="47">
+        <v>644.58000000000004</v>
+      </c>
+      <c r="J137" s="48">
+        <f t="shared" si="9"/>
+        <v>371.43000000000006</v>
+      </c>
+      <c r="K137" s="50"/>
+      <c r="L137" s="51"/>
+    </row>
+    <row r="138" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E138" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F138" s="45"/>
+      <c r="G138" s="47">
+        <v>657.22</v>
+      </c>
+      <c r="H138" s="48">
+        <f t="shared" si="8"/>
+        <v>384.07000000000005</v>
+      </c>
+      <c r="I138" s="47">
+        <v>644.54999999999995</v>
+      </c>
+      <c r="J138" s="48">
+        <f t="shared" si="9"/>
+        <v>371.4</v>
+      </c>
+      <c r="K138" s="50"/>
+      <c r="L138" s="51"/>
+    </row>
+    <row r="139" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E139" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F139" s="45"/>
+      <c r="G139" s="47">
+        <v>653.79</v>
+      </c>
+      <c r="H139" s="48">
+        <f t="shared" si="8"/>
+        <v>380.64</v>
+      </c>
+      <c r="I139" s="47">
+        <v>640.92999999999995</v>
+      </c>
+      <c r="J139" s="48">
+        <f t="shared" si="9"/>
+        <v>367.78</v>
+      </c>
+      <c r="K139" s="50"/>
+      <c r="L139" s="51"/>
+    </row>
+    <row r="140" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E140" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F140" s="45"/>
+      <c r="G140" s="47">
+        <v>308.5</v>
+      </c>
+      <c r="H140" s="48">
+        <f t="shared" si="8"/>
+        <v>35.350000000000023</v>
+      </c>
+      <c r="I140" s="47">
+        <v>295.68</v>
+      </c>
+      <c r="J140" s="48">
+        <f t="shared" si="9"/>
+        <v>22.53000000000003</v>
+      </c>
+      <c r="K140" s="50"/>
+      <c r="L140" s="51"/>
+    </row>
+    <row r="141" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E141" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="F141" s="45"/>
+      <c r="G141" s="47">
+        <v>655.57</v>
+      </c>
+      <c r="H141" s="48">
+        <f t="shared" si="8"/>
+        <v>382.42000000000007</v>
+      </c>
+      <c r="I141" s="47">
+        <v>642.80999999999995</v>
+      </c>
+      <c r="J141" s="48">
+        <f t="shared" si="9"/>
+        <v>369.65999999999997</v>
+      </c>
+      <c r="K141" s="50"/>
+      <c r="L141" s="51"/>
+    </row>
+    <row r="142" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E142" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F142" s="45"/>
+      <c r="G142" s="47">
+        <v>308.58</v>
+      </c>
+      <c r="H142" s="48">
+        <f t="shared" si="8"/>
+        <v>35.430000000000007</v>
+      </c>
+      <c r="I142" s="47">
+        <v>295.72000000000003</v>
+      </c>
+      <c r="J142" s="48">
+        <f t="shared" si="9"/>
+        <v>22.57000000000005</v>
+      </c>
+      <c r="K142" s="50"/>
+      <c r="L142" s="51"/>
+    </row>
+    <row r="143" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="E143" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F143" s="46"/>
+      <c r="G143" s="47">
+        <v>658.21</v>
+      </c>
+      <c r="H143" s="48">
+        <f t="shared" si="8"/>
+        <v>385.06000000000006</v>
+      </c>
+      <c r="I143" s="47">
+        <v>645.6</v>
+      </c>
+      <c r="J143" s="48">
+        <f t="shared" si="9"/>
+        <v>372.45000000000005</v>
+      </c>
+      <c r="K143" s="50"/>
+      <c r="L143" s="51"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="G121:J121"/>
+    <mergeCell ref="A122:C128"/>
+    <mergeCell ref="F122:F143"/>
+    <mergeCell ref="K122:L122"/>
+    <mergeCell ref="G123:H123"/>
+    <mergeCell ref="I123:J123"/>
+    <mergeCell ref="K123:L143"/>
+    <mergeCell ref="G92:J92"/>
+    <mergeCell ref="A93:C99"/>
+    <mergeCell ref="F93:F114"/>
+    <mergeCell ref="K93:L93"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="I94:J94"/>
+    <mergeCell ref="K94:L114"/>
+    <mergeCell ref="G63:J63"/>
+    <mergeCell ref="A64:C70"/>
+    <mergeCell ref="F64:F85"/>
+    <mergeCell ref="K64:L64"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="I65:J65"/>
+    <mergeCell ref="K65:L85"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="A36:C42"/>
+    <mergeCell ref="F36:F57"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="K37:L57"/>
+    <mergeCell ref="F8:F29"/>
+    <mergeCell ref="K9:L29"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="A8:C14"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:N21"/>
   <sheetViews>
@@ -5663,10 +8552,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="39"/>
+      <c r="C3" s="41"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
@@ -5771,11 +8660,11 @@
       <c r="N9" s="14"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
       <c r="H12" t="s">
         <v>50</v>
       </c>
@@ -5799,39 +8688,39 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5847,12 +8736,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:F31"/>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7367,8 +10256,8 @@
       <c r="K31" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
       <c r="N31" s="21" t="s">
         <v>94</v>
       </c>
@@ -7428,8 +10317,8 @@
       <c r="K32" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="L32" s="40"/>
-      <c r="M32" s="40"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
       <c r="N32" s="21">
         <v>0</v>
       </c>
@@ -7489,8 +10378,8 @@
       <c r="K33" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="L33" s="40"/>
-      <c r="M33" s="40"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
       <c r="N33" s="21">
         <v>0</v>
       </c>
@@ -7831,9 +10720,9 @@
       <c r="R38" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="S38" s="41"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="41"/>
+      <c r="S38" s="28"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="28"/>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
@@ -7890,9 +10779,9 @@
       <c r="R39" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="S39" s="41"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="41"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
     </row>
     <row r="40" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">

</xml_diff>